<commit_message>
Updated matrix column names
</commit_message>
<xml_diff>
--- a/input/Extra 400 1a.xlsx
+++ b/input/Extra 400 1a.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Code\dronelab\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E927B8-1C1C-43DF-B7F7-CE97E724C6C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Arahama 1 (1a)" sheetId="1" r:id="rId1"/>
@@ -23,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="10">
   <si>
     <t>Simulation</t>
   </si>
@@ -45,11 +44,20 @@
   <si>
     <t>Batch ID</t>
   </si>
+  <si>
+    <t>Social</t>
+  </si>
+  <si>
+    <t>Antisocial</t>
+  </si>
+  <si>
+    <t>WiFi Range</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -363,11 +371,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -392,16 +400,16 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2710,7 +2718,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4753,7 +4761,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6796,7 +6804,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F101"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>